<commit_message>
add missing blank EH4780 and EH4781 to run1 Ct+Tryp
</commit_message>
<xml_diff>
--- a/metadata/rawfiles_description_run1.xlsx
+++ b/metadata/rawfiles_description_run1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariiac/bioinf/immunohub/storage/mariiac/msms_figures/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED4DE97-810B-E64C-A588-3F5C354E10AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72E1AB4-2AC7-204E-B79F-DD000FB2039C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17680" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3234" uniqueCount="1360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3240" uniqueCount="1362">
   <si>
     <t>Rawfilenumber</t>
   </si>
@@ -4108,6 +4108,12 @@
   </si>
   <si>
     <t>Ct+Tryp</t>
+  </si>
+  <si>
+    <t>EH4780</t>
+  </si>
+  <si>
+    <t>EH4781</t>
   </si>
 </sst>
 </file>
@@ -15662,10 +15668,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C342"/>
+  <dimension ref="A1:C344"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G339" sqref="G339"/>
+    <sheetView tabSelected="1" topLeftCell="A318" workbookViewId="0">
+      <selection activeCell="F330" sqref="F330"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19436,6 +19442,28 @@
         <v>1359</v>
       </c>
     </row>
+    <row r="343" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A343" s="1" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B343" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C343" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A344" s="1" t="s">
+        <v>1361</v>
+      </c>
+      <c r="B344" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C344" t="s">
+        <v>1359</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>